<commit_message>
importadors els 4 fets , expresions regulars arreglat algun bug
</commit_message>
<xml_diff>
--- a/Gsport/Gsport/FitxersImport/Equips.xlsx
+++ b/Gsport/Gsport/FitxersImport/Equips.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>nom</t>
   </si>
@@ -31,9 +31,6 @@
     <t>id_entrenador</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Alevi A</t>
   </si>
   <si>
@@ -56,6 +53,27 @@
   </si>
   <si>
     <t>Pre-Benjami B</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -466,7 +484,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -497,7 +515,7 @@
     </row>
     <row r="2" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="10">
         <v>3</v>
@@ -506,7 +524,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6">
         <v>0</v>
@@ -514,7 +532,7 @@
     </row>
     <row r="3" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="10">
         <v>2</v>
@@ -523,7 +541,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
@@ -531,7 +549,7 @@
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="10">
         <v>1</v>
@@ -540,7 +558,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E4" s="7">
         <v>2</v>
@@ -548,7 +566,7 @@
     </row>
     <row r="5" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="10">
         <v>3</v>
@@ -557,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7">
         <v>3</v>
@@ -565,7 +583,7 @@
     </row>
     <row r="6" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="10">
         <v>3</v>
@@ -574,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E6" s="7">
         <v>4</v>
@@ -582,7 +600,7 @@
     </row>
     <row r="7" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="10">
         <v>4</v>
@@ -591,7 +609,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7">
         <v>5</v>
@@ -599,7 +617,7 @@
     </row>
     <row r="8" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="10">
         <v>4</v>
@@ -608,7 +626,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E8" s="7">
         <v>6</v>
@@ -616,7 +634,7 @@
     </row>
     <row r="9" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10">
         <v>1</v>
@@ -625,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E9" s="7">
         <v>7</v>

</xml_diff>